<commit_message>
updated GPIO for Mikes motor control section
</commit_message>
<xml_diff>
--- a/docs/pi_hat/GPIO_Pinout.xlsx
+++ b/docs/pi_hat/GPIO_Pinout.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Graeme\Desktop\solar_tracking_project\Hardware\pi_hat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Glen.Nicholls\Desktop\solar_tracking_project\docs\pi_hat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B3C88A-23DB-4710-810D-18E1FA081FF2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{5B4E5AD1-9CC3-496A-B7F0-65442161F04A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11568"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
   <si>
     <t>Component Pin</t>
   </si>
@@ -71,9 +70,6 @@
     <t>Elevation B</t>
   </si>
   <si>
-    <t>ADC</t>
-  </si>
-  <si>
     <t>CS</t>
   </si>
   <si>
@@ -98,9 +94,6 @@
     <t>ADC 13</t>
   </si>
   <si>
-    <t>RTC</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -137,9 +130,6 @@
     <t>PA7_PCINT7</t>
   </si>
   <si>
-    <t>AT tiny</t>
-  </si>
-  <si>
     <t>AT 7</t>
   </si>
   <si>
@@ -170,13 +160,64 @@
     <t>PA1_FAULT</t>
   </si>
   <si>
-    <t>Motor Control (Mike will have to fill this in)</t>
+    <t>L297</t>
+  </si>
+  <si>
+    <t>AZIMUTH_EN</t>
+  </si>
+  <si>
+    <t>ELEVATION_EN</t>
+  </si>
+  <si>
+    <t>RESET_N</t>
+  </si>
+  <si>
+    <t>CLOCK_N</t>
+  </si>
+  <si>
+    <t>DIRECTION</t>
+  </si>
+  <si>
+    <t>L297_1</t>
+  </si>
+  <si>
+    <t>L297_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> enable for azimuth motor driver</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> enable for elevation motor driver </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shared between both L297 driver chips </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shared between both L297 driver chips</t>
+  </si>
+  <si>
+    <t>Limit Switches</t>
+  </si>
+  <si>
+    <t>LIM_SW</t>
+  </si>
+  <si>
+    <t>MCP3008 ADC</t>
+  </si>
+  <si>
+    <t>DS3231 RTC</t>
+  </si>
+  <si>
+    <t>ATTiny84 Microcontroller</t>
+  </si>
+  <si>
+    <t>L297 Motor Control</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -246,11 +287,11 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -572,23 +613,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD125D1-636B-4535-A95A-3A65B99A69ED}">
-  <dimension ref="A1:E30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" customWidth="1"/>
+    <col min="5" max="5" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -602,10 +643,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -614,11 +655,11 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3">
@@ -628,10 +669,10 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -645,10 +686,10 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -662,10 +703,10 @@
         <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -679,24 +720,24 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>19</v>
@@ -705,12 +746,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>38</v>
@@ -719,12 +760,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>35</v>
@@ -733,12 +774,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>40</v>
@@ -747,21 +788,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -770,15 +811,15 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -787,24 +828,24 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16">
         <v>36</v>
@@ -813,15 +854,15 @@
         <v>16</v>
       </c>
       <c r="E16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
       </c>
       <c r="C17">
         <v>22</v>
@@ -830,15 +871,15 @@
         <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C18">
         <v>18</v>
@@ -847,15 +888,15 @@
         <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C19">
         <v>16</v>
@@ -864,15 +905,15 @@
         <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C20">
         <v>32</v>
@@ -881,15 +922,15 @@
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C21">
         <v>24</v>
@@ -898,15 +939,15 @@
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C22">
         <v>26</v>
@@ -915,76 +956,143 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24">
+        <v>15</v>
+      </c>
+      <c r="D24">
+        <v>22</v>
+      </c>
+      <c r="E24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25">
+        <v>13</v>
+      </c>
+      <c r="D25">
+        <v>27</v>
+      </c>
+      <c r="E25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C24">
+      <c r="C26">
         <v>31</v>
       </c>
-      <c r="D24">
+      <c r="D26">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C25">
+      <c r="E26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27">
         <v>21</v>
       </c>
-      <c r="D25">
+      <c r="D27">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C26">
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28">
         <v>28</v>
       </c>
-      <c r="D26">
+      <c r="D28">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C27">
-        <v>15</v>
-      </c>
-      <c r="D27">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C28">
-        <v>13</v>
-      </c>
-      <c r="D28">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C29">
+      <c r="E28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
         <v>11</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C30">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
         <v>12</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A29:E29"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="A2:E2"/>

</xml_diff>